<commit_message>
Event Summary generated output
for CIFMM-2321
</commit_message>
<xml_diff>
--- a/output/EventSummary/practitioner-dh-base-1.xlsx
+++ b/output/EventSummary/practitioner-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="442">
   <si>
     <t>Path</t>
   </si>
@@ -967,33 +967,33 @@
 </t>
   </si>
   <si>
-    <t>Name of a human - parts and usage</t>
-  </si>
-  <si>
-    <t>A human's name with the ability to identify parts and usage.</t>
-  </si>
-  <si>
-    <t>Names may be changed, or repudiated, or people may have different names in different contexts. Names may be divided into parts of different type that have variable significance depending on context, though the division into parts does not always matter. With personal names, the different parts may or may not be imbued with some implicit meaning; various cultures associate different importance with the name parts and the degree to which systems must care about name parts around the world varies widely.</t>
+    <t>The name(s) associated with the practitioner</t>
+  </si>
+  <si>
+    <t>The name(s) associated with the practitioner.</t>
+  </si>
+  <si>
+    <t>The selection of the use property should ensure that there is a single usual name specified, and others use the nickname (alias), old, or other values as appropriate.++In general select the value to be used in the ResourceReference.display based on this:++1. There is more than 1 name+2. Use = usual+3. Period is current to the date of the usage+4. Use = official+5. Other order as decided by internal business rules.</t>
   </si>
   <si>
     <t>The name(s) that a Practitioner is known by. Where there are multiple, the name that the practitioner is usually known as should be used in the display.</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-inv-dh-humn-01:The name shall at least have text or a family name or a given name {name.text.exists() or name.family.exists() or name.given.exists()}</t>
-  </si>
-  <si>
-    <t>XPN</t>
-  </si>
-  <si>
-    <t>EN (actually, PN)</t>
-  </si>
-  <si>
-    <t>ProviderName</t>
+    <t>XCN Components</t>
+  </si>
+  <si>
+    <t>./name</t>
+  </si>
+  <si>
+    <t>./PreferredName (GivenNames, FamilyName, TitleCode)</t>
   </si>
   <si>
     <t>Practitioner.telecom</t>
@@ -1602,7 +1602,7 @@
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="43.9296875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="99.6875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="50.04296875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="51.21484375" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="23.1640625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -10978,7 +10978,7 @@
         <v>40</v>
       </c>
       <c r="I85" t="s" s="2">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="J85" t="s" s="2">
         <v>301</v>
@@ -11051,19 +11051,19 @@
         <v>42</v>
       </c>
       <c r="AH85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="AI85" t="s" s="2">
+      <c r="AK85" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AJ85" t="s" s="2">
+      <c r="AL85" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AK85" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="AL85" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>40</v>
@@ -11071,7 +11071,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11094,19 +11094,19 @@
         <v>53</v>
       </c>
       <c r="J86" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K86" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="L86" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="K86" t="s" s="2">
+      <c r="M86" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="L86" t="s" s="2">
+      <c r="N86" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="M86" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>40</v>
@@ -11155,7 +11155,7 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -11170,13 +11170,13 @@
         <v>40</v>
       </c>
       <c r="AJ86" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AK86" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AL86" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AK86" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="AL86" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="AM86" t="s" s="2">
         <v>40</v>
@@ -11184,7 +11184,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11207,19 +11207,19 @@
         <v>53</v>
       </c>
       <c r="J87" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L87" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="K87" t="s" s="2">
+      <c r="M87" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="L87" t="s" s="2">
+      <c r="N87" t="s" s="2">
         <v>323</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="N87" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="O87" t="s" s="2">
         <v>40</v>
@@ -11268,7 +11268,7 @@
         <v>40</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>41</v>
@@ -11283,13 +11283,13 @@
         <v>40</v>
       </c>
       <c r="AJ87" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="AL87" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="AK87" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="AL87" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="AM87" t="s" s="2">
         <v>40</v>
@@ -11297,7 +11297,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11323,14 +11323,14 @@
         <v>71</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O88" t="s" s="2">
         <v>40</v>
@@ -11358,49 +11358,49 @@
         <v>138</v>
       </c>
       <c r="X88" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
         <v>333</v>
       </c>
-      <c r="Y88" t="s" s="2">
+      <c r="AK88" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="Z88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE88" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="AF88" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG88" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ88" t="s" s="2">
+      <c r="AL88" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="AK88" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="AL88" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="AM88" t="s" s="2">
         <v>40</v>
@@ -11408,7 +11408,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11431,17 +11431,17 @@
         <v>53</v>
       </c>
       <c r="J89" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L89" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="K89" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>341</v>
       </c>
       <c r="M89" s="2"/>
       <c r="N89" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="O89" t="s" s="2">
         <v>40</v>
@@ -11490,7 +11490,7 @@
         <v>40</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>41</v>
@@ -11505,13 +11505,13 @@
         <v>40</v>
       </c>
       <c r="AJ89" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AL89" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="AK89" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="AL89" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="AM89" t="s" s="2">
         <v>40</v>
@@ -11519,7 +11519,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11542,17 +11542,17 @@
         <v>40</v>
       </c>
       <c r="J90" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="K90" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="L90" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="K90" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="L90" t="s" s="2">
-        <v>349</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="O90" t="s" s="2">
         <v>40</v>
@@ -11601,7 +11601,7 @@
         <v>40</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>41</v>
@@ -11619,10 +11619,10 @@
         <v>40</v>
       </c>
       <c r="AK90" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM90" t="s" s="2">
         <v>40</v>
@@ -11630,7 +11630,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11653,13 +11653,13 @@
         <v>40</v>
       </c>
       <c r="J91" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="L91" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="K91" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="L91" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -11698,7 +11698,7 @@
         <v>40</v>
       </c>
       <c r="AA91" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AB91" s="2"/>
       <c r="AC91" t="s" s="2">
@@ -11708,7 +11708,7 @@
         <v>113</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>41</v>
@@ -11720,16 +11720,16 @@
         <v>40</v>
       </c>
       <c r="AI91" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AK91" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AJ91" t="s" s="2">
+      <c r="AL91" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AK91" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AL91" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="AM91" t="s" s="2">
         <v>40</v>
@@ -11737,7 +11737,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -11846,7 +11846,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -11957,11 +11957,11 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" t="s" s="2">
@@ -11986,7 +11986,7 @@
         <v>104</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="M94" t="s" s="2">
         <v>101</v>
@@ -12039,7 +12039,7 @@
         <v>40</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>41</v>
@@ -12068,7 +12068,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -12094,14 +12094,14 @@
         <v>108</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="O95" t="s" s="2">
         <v>40</v>
@@ -12150,7 +12150,7 @@
         <v>40</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>41</v>
@@ -12168,7 +12168,7 @@
         <v>40</v>
       </c>
       <c r="AK95" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AL95" t="s" s="2">
         <v>40</v>
@@ -12179,7 +12179,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -12205,10 +12205,10 @@
         <v>144</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
@@ -12235,52 +12235,52 @@
         <v>40</v>
       </c>
       <c r="W96" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y96" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="X96" t="s" s="2">
+      <c r="Z96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AL96" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="Y96" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="Z96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE96" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="AF96" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG96" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK96" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AL96" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="AM96" t="s" s="2">
         <v>40</v>
@@ -12288,7 +12288,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -12314,14 +12314,14 @@
         <v>195</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M97" s="2"/>
       <c r="N97" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="O97" t="s" s="2">
         <v>40</v>
@@ -12370,7 +12370,7 @@
         <v>40</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AF97" t="s" s="2">
         <v>41</v>
@@ -12388,10 +12388,10 @@
         <v>40</v>
       </c>
       <c r="AK97" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AL97" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AM97" t="s" s="2">
         <v>40</v>
@@ -12399,7 +12399,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -12425,10 +12425,10 @@
         <v>203</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -12479,7 +12479,7 @@
         <v>40</v>
       </c>
       <c r="AE98" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AF98" t="s" s="2">
         <v>41</v>
@@ -12497,7 +12497,7 @@
         <v>40</v>
       </c>
       <c r="AK98" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AL98" t="s" s="2">
         <v>40</v>
@@ -12508,7 +12508,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B99" t="s" s="2">
         <v>231</v>
@@ -12533,13 +12533,13 @@
         <v>40</v>
       </c>
       <c r="J99" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -12590,7 +12590,7 @@
         <v>40</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>41</v>
@@ -12602,16 +12602,16 @@
         <v>40</v>
       </c>
       <c r="AI99" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AJ99" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AK99" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AJ99" t="s" s="2">
+      <c r="AL99" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AK99" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AL99" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="AM99" t="s" s="2">
         <v>40</v>
@@ -12619,7 +12619,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -12728,7 +12728,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -12839,11 +12839,11 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" t="s" s="2">
@@ -12868,7 +12868,7 @@
         <v>104</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="M102" t="s" s="2">
         <v>101</v>
@@ -12921,7 +12921,7 @@
         <v>40</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>41</v>
@@ -12950,7 +12950,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -12976,14 +12976,14 @@
         <v>108</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="M103" s="2"/>
       <c r="N103" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="O103" t="s" s="2">
         <v>40</v>
@@ -13032,7 +13032,7 @@
         <v>40</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>41</v>
@@ -13044,13 +13044,13 @@
         <v>40</v>
       </c>
       <c r="AI103" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AJ103" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK103" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AL103" t="s" s="2">
         <v>40</v>
@@ -13061,7 +13061,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -13170,7 +13170,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13281,7 +13281,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -13394,7 +13394,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13420,7 +13420,7 @@
         <v>144</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L107" t="s" s="2">
         <v>146</v>
@@ -13507,7 +13507,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13616,7 +13616,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -13727,7 +13727,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -13840,7 +13840,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -13953,7 +13953,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -13979,7 +13979,7 @@
         <v>65</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L112" t="s" s="2">
         <v>219</v>
@@ -14064,7 +14064,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -14090,7 +14090,7 @@
         <v>123</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L113" t="s" s="2">
         <v>186</v>
@@ -14175,7 +14175,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -14284,7 +14284,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -14395,7 +14395,7 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -14421,10 +14421,10 @@
         <v>144</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
@@ -14451,52 +14451,52 @@
         <v>40</v>
       </c>
       <c r="W116" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="X116" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y116" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="X116" t="s" s="2">
+      <c r="Z116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE116" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AF116" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG116" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ116" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK116" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AL116" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="Y116" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="Z116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE116" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="AF116" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG116" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ116" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK116" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AL116" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="AM116" t="s" s="2">
         <v>40</v>
@@ -14504,7 +14504,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -14613,7 +14613,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -14724,7 +14724,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -14837,7 +14837,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -14863,7 +14863,7 @@
         <v>123</v>
       </c>
       <c r="K120" t="s" s="2">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L120" t="s" s="2">
         <v>167</v>
@@ -14950,7 +14950,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -14976,14 +14976,14 @@
         <v>195</v>
       </c>
       <c r="K121" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L121" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M121" s="2"/>
       <c r="N121" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="O121" t="s" s="2">
         <v>40</v>
@@ -15032,7 +15032,7 @@
         <v>40</v>
       </c>
       <c r="AE121" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AF121" t="s" s="2">
         <v>41</v>
@@ -15050,10 +15050,10 @@
         <v>40</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AL121" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AM121" t="s" s="2">
         <v>40</v>
@@ -15061,7 +15061,7 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -15087,10 +15087,10 @@
         <v>203</v>
       </c>
       <c r="K122" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L122" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
@@ -15141,7 +15141,7 @@
         <v>40</v>
       </c>
       <c r="AE122" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AF122" t="s" s="2">
         <v>41</v>
@@ -15159,7 +15159,7 @@
         <v>40</v>
       </c>
       <c r="AK122" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AL122" t="s" s="2">
         <v>40</v>
@@ -15170,7 +15170,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -15279,7 +15279,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -15390,7 +15390,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -15416,13 +15416,13 @@
         <v>123</v>
       </c>
       <c r="K125" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L125" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="M125" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="L125" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="M125" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="N125" s="2"/>
       <c r="O125" t="s" s="2">
@@ -15472,7 +15472,7 @@
         <v>40</v>
       </c>
       <c r="AE125" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AF125" t="s" s="2">
         <v>41</v>
@@ -15481,7 +15481,7 @@
         <v>52</v>
       </c>
       <c r="AH125" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AI125" t="s" s="2">
         <v>40</v>
@@ -15501,7 +15501,7 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -15527,13 +15527,13 @@
         <v>108</v>
       </c>
       <c r="K126" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="L126" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="M126" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="L126" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="M126" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="N126" s="2"/>
       <c r="O126" t="s" s="2">
@@ -15583,7 +15583,7 @@
         <v>40</v>
       </c>
       <c r="AE126" t="s" s="2">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AF126" t="s" s="2">
         <v>41</v>
@@ -15601,7 +15601,7 @@
         <v>40</v>
       </c>
       <c r="AK126" t="s" s="2">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AL126" t="s" s="2">
         <v>40</v>
@@ -15612,7 +15612,7 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -15638,13 +15638,13 @@
         <v>123</v>
       </c>
       <c r="K127" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="L127" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="M127" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="L127" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="M127" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="N127" s="2"/>
       <c r="O127" t="s" s="2">
@@ -15652,7 +15652,7 @@
       </c>
       <c r="P127" s="2"/>
       <c r="Q127" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="R127" t="s" s="2">
         <v>40</v>
@@ -15694,7 +15694,7 @@
         <v>40</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>41</v>
@@ -15723,7 +15723,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -15749,16 +15749,16 @@
         <v>144</v>
       </c>
       <c r="K128" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="L128" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="M128" t="s" s="2">
         <v>436</v>
       </c>
-      <c r="L128" t="s" s="2">
+      <c r="N128" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="M128" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="N128" t="s" s="2">
-        <v>439</v>
       </c>
       <c r="O128" t="s" s="2">
         <v>40</v>
@@ -15787,7 +15787,7 @@
       </c>
       <c r="X128" s="2"/>
       <c r="Y128" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="Z128" t="s" s="2">
         <v>40</v>
@@ -15805,7 +15805,7 @@
         <v>40</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>41</v>
@@ -15820,13 +15820,13 @@
         <v>40</v>
       </c>
       <c r="AJ128" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AK128" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AL128" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="AK128" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="AL128" t="s" s="2">
-        <v>443</v>
       </c>
       <c r="AM128" t="s" s="2">
         <v>40</v>

</xml_diff>